<commit_message>
Excel diagram fixed girls :)
</commit_message>
<xml_diff>
--- a/I-R_Diagram/DiagramTables.xlsx
+++ b/I-R_Diagram/DiagramTables.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maria\OneDrive\Imágenes\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maria\git\OncologyDataBase\I-R_Diagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D3A90338-B3A4-4AB1-B39A-A8B057A2968C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{874FB22B-B84B-44AE-AC39-26B2DD7A2AEE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="29">
   <si>
     <t>PATIENT</t>
   </si>
@@ -79,9 +79,6 @@
   </si>
   <si>
     <t>TREATMENT</t>
-  </si>
-  <si>
-    <t>effects</t>
   </si>
   <si>
     <t>startDate</t>
@@ -699,8 +696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:K53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -953,82 +950,67 @@
       <c r="E27" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F27" s="2" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B28" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B29" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B30" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B31" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="32" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="33" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
@@ -1042,71 +1024,71 @@
         <v>12</v>
       </c>
       <c r="D34" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B35" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B36" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B37" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B38" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B41" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C41" s="6"/>
       <c r="D41" s="6"/>
@@ -1116,10 +1098,10 @@
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B42" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C42" s="19" t="s">
         <v>24</v>
-      </c>
-      <c r="C42" s="19" t="s">
-        <v>25</v>
       </c>
       <c r="D42" s="10" t="s">
         <v>13</v>
@@ -1128,18 +1110,18 @@
         <v>1</v>
       </c>
       <c r="I42" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="J42" s="22" t="s">
         <v>26</v>
-      </c>
-      <c r="J42" s="22" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B43" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C43" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D43" s="1"/>
       <c r="H43" s="1"/>
@@ -1148,10 +1130,10 @@
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B44" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D44" s="1"/>
       <c r="H44" s="1"/>
@@ -1160,10 +1142,10 @@
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B45" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C45" s="21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D45" s="1"/>
       <c r="H45" s="1"/>
@@ -1177,7 +1159,7 @@
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B48" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.3">
@@ -1188,7 +1170,7 @@
         <v>12</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Interface created Methods in process One week more, one week less :)
</commit_message>
<xml_diff>
--- a/I-R_Diagram/DiagramTables.xlsx
+++ b/I-R_Diagram/DiagramTables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maria\git\OncologyDataBase\I-R_Diagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{874FB22B-B84B-44AE-AC39-26B2DD7A2AEE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3AC29B5-C97F-4590-9375-9FFFDC37C280}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="30">
   <si>
     <t>PATIENT</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>member</t>
+  </si>
+  <si>
+    <t>n-n</t>
   </si>
 </sst>
 </file>
@@ -172,13 +175,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FFC65911"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC65911"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -332,7 +335,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -366,7 +369,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
@@ -379,7 +381,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -696,8 +701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:K53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -710,6 +715,7 @@
     <col min="7" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="14.109375" customWidth="1"/>
     <col min="9" max="9" width="15.109375" customWidth="1"/>
+    <col min="10" max="11" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:11" x14ac:dyDescent="0.3">
@@ -881,56 +887,71 @@
       <c r="B18" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="17" t="s">
+      <c r="G18" s="16" t="s">
         <v>10</v>
+      </c>
+      <c r="J18" s="24" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B19" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="15" t="s">
         <v>12</v>
       </c>
       <c r="D19" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G19" s="18" t="s">
+      <c r="G19" s="17" t="s">
         <v>11</v>
       </c>
       <c r="H19" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="J19" s="15"/>
-      <c r="K19" s="15"/>
+      <c r="J19" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="K19" s="23" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
-      <c r="C20" s="16"/>
+      <c r="C20" s="15"/>
       <c r="D20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
+      <c r="J20" s="22"/>
+      <c r="K20" s="22"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
-      <c r="C21" s="16"/>
+      <c r="C21" s="15"/>
       <c r="D21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
+      <c r="J21" s="22"/>
+      <c r="K21" s="22"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B22" s="1"/>
-      <c r="C22" s="16"/>
+      <c r="C22" s="15"/>
       <c r="D22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="22"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B23" s="1"/>
-      <c r="C23" s="16"/>
+      <c r="C23" s="15"/>
       <c r="D23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
+      <c r="J23" s="22"/>
+      <c r="K23" s="22"/>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B26" s="13" t="s">
@@ -1092,7 +1113,7 @@
       </c>
       <c r="C41" s="6"/>
       <c r="D41" s="6"/>
-      <c r="H41" s="17" t="s">
+      <c r="H41" s="16" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1100,19 +1121,19 @@
       <c r="B42" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C42" s="19" t="s">
+      <c r="C42" s="18" t="s">
         <v>24</v>
       </c>
       <c r="D42" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="H42" s="18" t="s">
+      <c r="H42" s="17" t="s">
         <v>1</v>
       </c>
       <c r="I42" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="J42" s="22" t="s">
+      <c r="J42" s="21" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1120,7 +1141,7 @@
       <c r="B43" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C43" s="20" t="s">
+      <c r="C43" s="19" t="s">
         <v>18</v>
       </c>
       <c r="D43" s="1"/>
@@ -1144,7 +1165,7 @@
       <c r="B45" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C45" s="21" t="s">
+      <c r="C45" s="20" t="s">
         <v>18</v>
       </c>
       <c r="D45" s="1"/>

</xml_diff>